<commit_message>
S03P31A205-92/feature/testcase : Update testcase
</commit_message>
<xml_diff>
--- a/산출물/테스트케이스_Photory.xlsx
+++ b/산출물/테스트케이스_Photory.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\multicampus\Desktop\3 자율플젝\문서\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\multicampus\Desktop\3 자율플젝\s03p31a205\산출물\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="60">
   <si>
     <t>테스트 케이스 (FINAL)</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -163,10 +163,6 @@
   </si>
   <si>
     <t>글쓰기, 내 글 수정</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>F</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -238,10 +234,6 @@
   </si>
   <si>
     <t>저장된 동화를 내 보관함에서 확인가능</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>F</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -521,6 +513,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -539,6 +537,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -547,15 +548,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -841,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -855,48 +847,48 @@
     <col min="7" max="7" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="15" customFormat="1" ht="27.6">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:10" s="14" customFormat="1" ht="27.6">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="18" thickBot="1"/>
     <row r="4" spans="1:10">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="14"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="B5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="8"/>
+      <c r="B5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10" ht="70.2" customHeight="1" thickBot="1">
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:10">
       <c r="B7" s="1"/>
@@ -991,7 +983,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1">
-      <c r="B12" s="16">
+      <c r="B12" s="6">
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1031,7 +1023,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" s="1" customFormat="1">
-      <c r="B14" s="16">
+      <c r="B14" s="6">
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1056,7 +1048,7 @@
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1">
-      <c r="B16" s="16"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1068,41 +1060,41 @@
     </row>
     <row r="18" spans="2:10" ht="18" thickBot="1"/>
     <row r="19" spans="2:10">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="14"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="17"/>
     </row>
     <row r="20" spans="2:10">
-      <c r="B20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="8"/>
+      <c r="B20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="2:10" ht="90" customHeight="1" thickBot="1">
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="13"/>
     </row>
     <row r="23" spans="2:10" ht="17.399999999999999" customHeight="1">
       <c r="B23" s="3" t="s">
@@ -1195,10 +1187,10 @@
         <v>34</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>4</v>
@@ -1213,52 +1205,52 @@
       <c r="B29" s="5"/>
     </row>
     <row r="30" spans="2:10">
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="14"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="17"/>
     </row>
     <row r="31" spans="2:10">
-      <c r="B31" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="8"/>
+      <c r="B31" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="10"/>
     </row>
     <row r="32" spans="2:10" ht="123.6" customHeight="1" thickBot="1">
-      <c r="B32" s="9"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="13"/>
     </row>
     <row r="33" spans="2:10" ht="17.399999999999999" customHeight="1">
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
     </row>
     <row r="34" spans="2:10" ht="19.2" customHeight="1">
       <c r="B34" s="3" t="s">
@@ -1279,151 +1271,151 @@
       <c r="G34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
     </row>
     <row r="35" spans="2:10" ht="19.2" customHeight="1">
       <c r="B35" s="5">
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="E35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
     </row>
     <row r="36" spans="2:10" ht="16.2" customHeight="1">
       <c r="B36" s="1">
         <v>2</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D36" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="F36" s="1" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
     </row>
     <row r="37" spans="2:10" ht="21" customHeight="1">
       <c r="B37" s="1">
         <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+    </row>
+    <row r="38" spans="2:10" ht="22.8" customHeight="1">
+      <c r="B38" s="6">
+        <v>4</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-    </row>
-    <row r="38" spans="2:10" ht="22.8" customHeight="1">
-      <c r="B38" s="16">
-        <v>4</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="F38" s="1" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
     </row>
     <row r="39" spans="2:10" ht="21" customHeight="1">
       <c r="B39" s="1"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="17"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
     </row>
     <row r="40" spans="2:10" ht="17.399999999999999" customHeight="1">
-      <c r="B40" s="16"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17"/>
+      <c r="B40" s="6"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
     </row>
     <row r="41" spans="2:10" ht="18" thickBot="1"/>
     <row r="42" spans="2:10">
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="14"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="17"/>
     </row>
     <row r="43" spans="2:10" ht="17.399999999999999" customHeight="1">
-      <c r="B43" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="8"/>
+      <c r="B43" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="10"/>
     </row>
     <row r="44" spans="2:10" ht="126" customHeight="1" thickBot="1">
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="13"/>
     </row>
     <row r="45" spans="2:10">
       <c r="B45" s="5"/>
@@ -1455,13 +1447,13 @@
         <v>1</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>23</v>
@@ -1475,16 +1467,16 @@
         <v>2</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>4</v>
@@ -1495,36 +1487,36 @@
         <v>3</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="E49" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7">
+      <c r="B50" s="6">
+        <v>4</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7">
-      <c r="B50" s="16">
-        <v>4</v>
-      </c>
-      <c r="C50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="F50" s="1" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>4</v>

</xml_diff>